<commit_message>
Cambios 27 marzo 23 1a parte
</commit_message>
<xml_diff>
--- a/1_data/datos_1_stocks.xlsx
+++ b/1_data/datos_1_stocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffbris/Desktop/22 Migración ASI/ENOE/SDEMT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffbris/Desktop/23 Migración ASI servicios/OIM_migracion_servicios/1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0194E528-E643-AF49-8C58-9BFA58D8CC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ADF036-DEA6-B841-B625-B8148D2E1641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="3000" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{D06A6A23-6A6C-CF40-8A55-C78D1710B4ED}"/>
+    <workbookView xWindow="6760" yWindow="3000" windowWidth="26840" windowHeight="15940" xr2:uid="{D06A6A23-6A6C-CF40-8A55-C78D1710B4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="UPMigratoria" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>International Migrant Stock 2020: Destination</t>
   </si>
   <si>
@@ -280,17 +277,20 @@
   <si>
     <t>Modelo de corrección de errores</t>
   </si>
+  <si>
+    <t>total_entradas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="###\ ###\ ##0;\-###\ ###\ ##0;\—;"/>
-    <numFmt numFmtId="170" formatCode="###\ ###\ ###\ ###\ ##0"/>
-    <numFmt numFmtId="173" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="###\ ###\ ##0;\-###\ ###\ ##0;\—;"/>
+    <numFmt numFmtId="166" formatCode="###\ ###\ ###\ ###\ ##0"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -538,12 +538,12 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -558,7 +558,7 @@
     <xf numFmtId="1" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
@@ -568,12 +568,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,19 +580,13 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,15 +601,14 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="13" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,9 +621,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -645,6 +632,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -966,81 +965,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7FA61A-A9F7-1847-A99E-389CE693DC99}">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -2773,7 +2772,7 @@
         <v>2021</v>
       </c>
       <c r="B32">
-        <v>25536881.288659796</v>
+        <v>25536881.2886598</v>
       </c>
       <c r="C32">
         <v>19136629</v>
@@ -2856,16 +2855,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2878,7 +2877,7 @@
       <c r="C2">
         <v>235679.14199999999</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2">
         <v>17220424</v>
       </c>
     </row>
@@ -2991,7 +2990,7 @@
       <c r="C12">
         <v>375644.81800000003</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12">
         <v>19747511</v>
       </c>
     </row>
@@ -3005,7 +3004,6 @@
       <c r="C13">
         <v>425725.58600000001</v>
       </c>
-      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -3017,7 +3015,6 @@
       <c r="C14">
         <v>459724.96</v>
       </c>
-      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -3029,7 +3026,6 @@
       <c r="C15">
         <v>438755.22100000002</v>
       </c>
-      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -3041,7 +3037,6 @@
       <c r="C16">
         <v>456331.19300000003</v>
       </c>
-      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -3053,7 +3048,6 @@
       <c r="C17">
         <v>500247.18599999999</v>
       </c>
-      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -3065,7 +3059,6 @@
       <c r="C18">
         <v>543435.49899999995</v>
       </c>
-      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -3077,7 +3070,6 @@
       <c r="C19">
         <v>543636.60400000005</v>
       </c>
-      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -3089,7 +3081,6 @@
       <c r="C20">
         <v>558303.83700000006</v>
       </c>
-      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -3101,7 +3092,6 @@
       <c r="C21">
         <v>522036.57299999997</v>
       </c>
-      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -3113,7 +3103,7 @@
       <c r="C22">
         <v>455639.136</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22">
         <v>21611963</v>
       </c>
     </row>
@@ -3124,7 +3114,6 @@
       <c r="B23">
         <v>20386.907843000001</v>
       </c>
-      <c r="D23" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3188,7 +3177,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>-8.3000000000000007</v>
@@ -3216,45 +3205,45 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C3" s="33">
+      <c r="C3" s="28">
         <f>+(C4-B4)/B4</f>
         <v>0.13574064451158593</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="28">
         <f>+D2/100</f>
         <v>-8.3000000000000004E-2</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="28">
         <f t="shared" ref="E3:K3" si="1">+E2/100</f>
         <v>6.3E-2</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="28">
         <f t="shared" si="1"/>
         <v>4.0999999999999995E-2</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="28">
         <f t="shared" si="1"/>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="28">
         <f t="shared" si="1"/>
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="28">
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="28">
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K3" s="33">
+      <c r="K3" s="28">
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="26">
+      <c r="B4" s="22">
         <v>65139134.1151338</v>
       </c>
       <c r="C4">
@@ -3262,87 +3251,87 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C5" s="29"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="28">
+      <c r="B6" s="23">
         <v>8166125</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="29">
         <f>+B6*(1+C3)</f>
         <v>9274600.0706621744</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="29">
         <f t="shared" ref="D6:K6" si="2">+C6*(1+D3)</f>
         <v>8504808.2647972144</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="29">
         <f t="shared" si="2"/>
         <v>9040611.1854794379</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="29">
         <f t="shared" si="2"/>
         <v>9411276.2440840937</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="29">
         <f t="shared" si="2"/>
         <v>9731259.6363829523</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="29">
         <f t="shared" si="2"/>
         <v>10003734.906201676</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="29">
         <f t="shared" si="2"/>
         <v>10253828.278856717</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="29">
         <f t="shared" si="2"/>
         <v>10510173.985828133</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="29">
         <f t="shared" si="2"/>
         <v>10772928.335473835</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G7" s="35">
+      <c r="G7" s="30">
         <f>+G6-F6</f>
         <v>319983.39229885861</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="30">
         <f t="shared" ref="H7:K7" si="3">+H6-G6</f>
         <v>272475.2698187232</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="30">
         <f t="shared" si="3"/>
         <v>250093.37265504152</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="30">
         <f t="shared" si="3"/>
         <v>256345.70697141625</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="30">
         <f t="shared" si="3"/>
         <v>262754.34964570217</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="30">
+      <c r="B10" s="25">
         <v>18533875.320545498</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="26">
         <v>18461147.610820901</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="26">
         <v>18566923.334562801</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="27">
         <v>18419215.8969195</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="26">
+      <c r="B11" s="22">
         <f>+SUM(B10:E10)</f>
         <v>73981162.162848696</v>
       </c>
@@ -3375,83 +3364,83 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="36">
+        <v>47</v>
+      </c>
+      <c r="F16" s="31">
         <f>+F3</f>
         <v>4.0999999999999995E-2</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="31">
         <f t="shared" ref="G16:K16" si="5">+G3</f>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="31">
         <f t="shared" si="5"/>
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="I16" s="36">
+      <c r="I16" s="31">
         <f t="shared" si="5"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J16" s="36">
+      <c r="J16" s="31">
         <f t="shared" si="5"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K16" s="36">
+      <c r="K16" s="31">
         <f t="shared" si="5"/>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="35">
+        <v>48</v>
+      </c>
+      <c r="F17" s="30">
         <f>+F6</f>
         <v>9411276.2440840937</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="30">
         <f t="shared" ref="G17:K17" si="6">+G6</f>
         <v>9731259.6363829523</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="30">
         <f t="shared" si="6"/>
         <v>10003734.906201676</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="30">
         <f t="shared" si="6"/>
         <v>10253828.278856717</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="30">
         <f t="shared" si="6"/>
         <v>10510173.985828133</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="30">
         <f t="shared" si="6"/>
         <v>10772928.335473835</v>
       </c>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="35">
+        <v>49</v>
+      </c>
+      <c r="G18" s="30">
         <f>+G7</f>
         <v>319983.39229885861</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="30">
         <f t="shared" ref="H18:K18" si="7">+H7</f>
         <v>272475.2698187232</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="30">
         <f t="shared" si="7"/>
         <v>250093.37265504152</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="30">
         <f t="shared" si="7"/>
         <v>256345.70697141625</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="30">
         <f t="shared" si="7"/>
         <v>262754.34964570217</v>
       </c>
@@ -3481,7 +3470,7 @@
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>11016981</v>
@@ -3493,7 +3482,7 @@
         <v>11504006</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N6">
         <v>11016981</v>
@@ -3507,7 +3496,7 @@
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>11093360</v>
@@ -3519,7 +3508,7 @@
         <v>11653775</v>
       </c>
       <c r="M7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N7">
         <v>11093360</v>
@@ -3533,7 +3522,7 @@
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>11120532</v>
@@ -3545,7 +3534,7 @@
         <v>11790756</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N8">
         <v>11120532</v>
@@ -3559,7 +3548,7 @@
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>11168899</v>
@@ -3575,7 +3564,7 @@
         <v>114052</v>
       </c>
       <c r="M9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N9">
         <v>11168899</v>
@@ -3589,7 +3578,7 @@
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10">
         <v>11208136</v>
@@ -3601,7 +3590,7 @@
         <v>12030678</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N10">
         <v>11208136</v>
@@ -3615,7 +3604,7 @@
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>11251306</v>
@@ -3627,7 +3616,7 @@
         <v>12140675</v>
       </c>
       <c r="M11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N11">
         <v>11251306</v>
@@ -3641,7 +3630,7 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>11292782</v>
@@ -3668,7 +3657,7 @@
         <v>2027</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N12">
         <v>11292782</v>
@@ -3682,7 +3671,7 @@
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>11334987</v>
@@ -3693,28 +3682,28 @@
       <c r="F13">
         <v>12346469</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="29">
         <f>+D9-D5</f>
         <v>114052</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="29">
         <f>+D13-D9</f>
         <v>166088</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="29">
         <f>+D17-D13</f>
         <v>167879</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="29">
         <f>+D21-D17</f>
         <v>167941</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K13" s="29">
         <f>+D25-D21</f>
         <v>167943</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N13">
         <v>11334987</v>
@@ -3728,7 +3717,7 @@
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>11376878</v>
@@ -3739,9 +3728,9 @@
       <c r="F14">
         <v>12444160</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="29"/>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>11376878</v>
@@ -3755,7 +3744,7 @@
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15">
         <v>11418905</v>
@@ -3766,9 +3755,9 @@
       <c r="F15">
         <v>12539135</v>
       </c>
-      <c r="H15" s="34"/>
+      <c r="H15" s="29"/>
       <c r="M15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N15">
         <v>11418905</v>
@@ -3782,7 +3771,7 @@
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <v>11460873</v>
@@ -3793,9 +3782,9 @@
       <c r="F16">
         <v>12631691</v>
       </c>
-      <c r="H16" s="34"/>
+      <c r="H16" s="29"/>
       <c r="M16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16">
         <v>11460873</v>
@@ -3809,7 +3798,7 @@
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>11502866</v>
@@ -3821,7 +3810,7 @@
         <v>12722163</v>
       </c>
       <c r="M17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N17">
         <v>11502866</v>
@@ -3835,7 +3824,7 @@
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>11544849</v>
@@ -3846,9 +3835,9 @@
       <c r="F18">
         <v>12810773</v>
       </c>
-      <c r="H18" s="34"/>
+      <c r="H18" s="29"/>
       <c r="M18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N18">
         <v>11544849</v>
@@ -3862,7 +3851,7 @@
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19">
         <v>11586836</v>
@@ -3873,9 +3862,9 @@
       <c r="F19">
         <v>12897729</v>
       </c>
-      <c r="H19" s="34"/>
+      <c r="H19" s="29"/>
       <c r="M19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N19">
         <v>11586836</v>
@@ -3889,7 +3878,7 @@
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>11628821</v>
@@ -3900,9 +3889,9 @@
       <c r="F20">
         <v>12983191</v>
       </c>
-      <c r="H20" s="34"/>
+      <c r="H20" s="29"/>
       <c r="M20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N20">
         <v>11628821</v>
@@ -3916,7 +3905,7 @@
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21">
         <v>11670807</v>
@@ -3928,7 +3917,7 @@
         <v>13067301</v>
       </c>
       <c r="M21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N21">
         <v>11670807</v>
@@ -3942,7 +3931,7 @@
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22">
         <v>11712793</v>
@@ -3953,9 +3942,9 @@
       <c r="F22">
         <v>13150176</v>
       </c>
-      <c r="H22" s="34"/>
+      <c r="H22" s="29"/>
       <c r="M22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N22">
         <v>11712793</v>
@@ -3969,7 +3958,7 @@
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23">
         <v>11754779</v>
@@ -3980,9 +3969,9 @@
       <c r="F23">
         <v>13231921</v>
       </c>
-      <c r="H23" s="34"/>
+      <c r="H23" s="29"/>
       <c r="M23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N23">
         <v>11754779</v>
@@ -3996,7 +3985,7 @@
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24">
         <v>11796764</v>
@@ -4007,9 +3996,9 @@
       <c r="F24">
         <v>13312622</v>
       </c>
-      <c r="H24" s="34"/>
+      <c r="H24" s="29"/>
       <c r="M24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N24">
         <v>11796764</v>
@@ -4023,7 +4012,7 @@
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25">
         <v>11838750</v>
@@ -4035,7 +4024,7 @@
         <v>13392360</v>
       </c>
       <c r="M25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N25">
         <v>11838750</v>
@@ -4056,7 +4045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FE690A-39EC-A246-975C-F22A53ECB7B8}">
   <dimension ref="C5:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34:I37"/>
     </sheetView>
   </sheetViews>
@@ -4064,729 +4053,729 @@
   <sheetData>
     <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>10.21116</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="29">
         <f>+EXP(D5)</f>
         <v>27205.107217291963</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>10.21205</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="29">
         <f>+EXP(H5)</f>
         <v>27229.330540495241</v>
       </c>
       <c r="L5">
         <v>10.18716</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="29">
         <f>+EXP(L5)</f>
         <v>26559.95740867393</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>10.190569999999999</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="29">
         <f t="shared" ref="E6:E24" si="0">+EXP(D6)</f>
         <v>26650.681460032698</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6">
         <v>10.17403</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="29">
         <f t="shared" ref="I6:I24" si="1">+EXP(H6)</f>
         <v>26213.50460780385</v>
       </c>
       <c r="L6">
         <v>10.17905</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="29">
         <f t="shared" ref="M6:M24" si="2">+EXP(L6)</f>
         <v>26345.427249724416</v>
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>10.178890000000001</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="29">
         <f t="shared" si="0"/>
         <v>26341.212318567963</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>10.17226</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="29">
         <f t="shared" si="1"/>
         <v>26167.14774257637</v>
       </c>
       <c r="L7">
         <v>10.24497</v>
       </c>
-      <c r="M7" s="34">
+      <c r="M7" s="29">
         <f t="shared" si="2"/>
         <v>28140.637922222402</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>10.16949</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="29">
         <f t="shared" si="0"/>
         <v>26094.765039655078</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>10.20219</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="29">
         <f t="shared" si="1"/>
         <v>26962.168614107515</v>
       </c>
       <c r="L8">
         <v>10.254569999999999</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="29">
         <f t="shared" si="2"/>
         <v>28412.088926355034</v>
       </c>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>10.163029999999999</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="29">
         <f t="shared" si="0"/>
         <v>25926.73617507386</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <v>10.148440000000001</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="29">
         <f t="shared" si="1"/>
         <v>25551.211210314344</v>
       </c>
       <c r="L9">
         <v>10.249169999999999</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="29">
         <f t="shared" si="2"/>
         <v>28259.077149767945</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>10.15828</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="29">
         <f t="shared" si="0"/>
         <v>25803.876201681338</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>10.20928</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="29">
         <f t="shared" si="1"/>
         <v>27154.00966247492</v>
       </c>
       <c r="L10">
         <v>10.256360000000001</v>
       </c>
-      <c r="M10" s="34">
+      <c r="M10" s="29">
         <f t="shared" si="2"/>
         <v>28462.992110291303</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11">
         <v>10.15489</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="29">
         <f t="shared" si="0"/>
         <v>25716.549164316886</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>10.250920000000001</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="29">
         <f t="shared" si="1"/>
         <v>28308.573831744838</v>
       </c>
       <c r="L11">
         <v>10.276949999999999</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="29">
         <f t="shared" si="2"/>
         <v>29055.120156933455</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>10.15244</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="29">
         <f t="shared" si="0"/>
         <v>25653.620737664289</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12">
         <v>10.25483</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="29">
         <f t="shared" si="1"/>
         <v>28419.477029887752</v>
       </c>
       <c r="L12">
         <v>10.286490000000001</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="29">
         <f t="shared" si="2"/>
         <v>29333.632394285651</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13">
         <v>10.15067</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="29">
         <f t="shared" si="0"/>
         <v>25608.253990374087</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13">
         <v>10.19272</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="29">
         <f t="shared" si="1"/>
         <v>26708.042065727117</v>
       </c>
       <c r="L13">
         <v>10.291309999999999</v>
       </c>
-      <c r="M13" s="34">
+      <c r="M13" s="29">
         <f t="shared" si="2"/>
         <v>29475.3617958912</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>10.1494</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="29">
         <f t="shared" si="0"/>
         <v>25575.752150842934</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14">
         <v>10.2037</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="29">
         <f t="shared" si="1"/>
         <v>27002.912242412553</v>
       </c>
       <c r="L14">
         <v>10.30001</v>
       </c>
-      <c r="M14" s="34">
+      <c r="M14" s="29">
         <f t="shared" si="2"/>
         <v>29732.91618056659</v>
       </c>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15">
         <v>10.148490000000001</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="29">
         <f t="shared" si="0"/>
         <v>25552.488802814401</v>
       </c>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15">
         <v>10.220409999999999</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="29">
         <f t="shared" si="1"/>
         <v>27457.921924453571</v>
       </c>
       <c r="L15">
         <v>10.31162</v>
       </c>
-      <c r="M15" s="34">
+      <c r="M15" s="29">
         <f t="shared" si="2"/>
         <v>30080.126996109684</v>
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16">
         <v>10.147830000000001</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="29">
         <f t="shared" si="0"/>
         <v>25535.629724312439</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16">
         <v>10.232989999999999</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="29">
         <f t="shared" si="1"/>
         <v>27805.52441776494</v>
       </c>
       <c r="L16">
         <v>10.32084</v>
       </c>
-      <c r="M16" s="34">
+      <c r="M16" s="29">
         <f t="shared" si="2"/>
         <v>30358.748237175794</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17">
         <v>10.147349999999999</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="29">
         <f t="shared" si="0"/>
         <v>25523.37556327866</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H17">
         <v>10.17108</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="29">
         <f t="shared" si="1"/>
         <v>26136.28871864493</v>
       </c>
       <c r="L17">
         <v>10.32884</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="29">
         <f t="shared" si="2"/>
         <v>30602.592298819476</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>10.14701</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="29">
         <f t="shared" si="0"/>
         <v>25514.699090671085</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18">
         <v>10.205019999999999</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="29">
         <f t="shared" si="1"/>
         <v>27038.579621864064</v>
       </c>
       <c r="L18">
         <v>10.33784</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="29">
         <f t="shared" si="2"/>
         <v>30879.258761092991</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>10.14676</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="29">
         <f t="shared" si="0"/>
         <v>25508.321213166339</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19">
         <v>10.232670000000001</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="29">
         <f t="shared" si="1"/>
         <v>27796.628073442305</v>
       </c>
       <c r="L19">
         <v>10.34751</v>
       </c>
-      <c r="M19" s="34">
+      <c r="M19" s="29">
         <f t="shared" si="2"/>
         <v>31179.309601008728</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>10.14659</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="29">
         <f t="shared" si="0"/>
         <v>25503.985167134437</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H20">
         <v>10.239750000000001</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="29">
         <f t="shared" si="1"/>
         <v>27994.126519712256</v>
       </c>
       <c r="L20">
         <v>10.356640000000001</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="29">
         <f t="shared" si="2"/>
         <v>31465.280166833389</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21">
         <v>10.146459999999999</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="29">
         <f t="shared" si="0"/>
         <v>25500.669864562034</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H21">
         <v>10.17698</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="29">
         <f t="shared" si="1"/>
         <v>26290.948620152056</v>
       </c>
       <c r="L21">
         <v>10.365460000000001</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="29">
         <f t="shared" si="2"/>
         <v>31744.03142389005</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22">
         <v>10.146369999999999</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="29">
         <f t="shared" si="0"/>
         <v>25498.374907548838</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H22">
         <v>10.198790000000001</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="29">
         <f t="shared" si="1"/>
         <v>26870.652905684008</v>
       </c>
       <c r="L22">
         <v>10.37452</v>
       </c>
-      <c r="M22" s="34">
+      <c r="M22" s="29">
         <f t="shared" si="2"/>
         <v>32032.939124260527</v>
       </c>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23">
         <v>10.1463</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="29">
         <f t="shared" si="0"/>
         <v>25496.590083774892</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H23">
         <v>10.22057</v>
       </c>
-      <c r="I23" s="34">
+      <c r="I23" s="29">
         <f t="shared" si="1"/>
         <v>27462.315543441659</v>
       </c>
       <c r="L23">
         <v>10.38374</v>
       </c>
-      <c r="M23" s="34">
+      <c r="M23" s="29">
         <f t="shared" si="2"/>
         <v>32329.64855154949</v>
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24">
         <v>10.14625</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="29">
         <f t="shared" si="0"/>
         <v>25495.315286140911</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H24">
         <v>10.230230000000001</v>
       </c>
-      <c r="I24" s="34">
+      <c r="I24" s="29">
         <f t="shared" si="1"/>
         <v>27728.886978687318</v>
       </c>
       <c r="L24">
         <v>10.39283</v>
       </c>
-      <c r="M24" s="34">
+      <c r="M24" s="29">
         <f t="shared" si="2"/>
         <v>32624.86478188977</v>
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="E28" s="35">
+      <c r="E28" s="30">
         <f>+E8</f>
         <v>26094.765039655078</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I28" s="30">
         <f>+I8</f>
         <v>26962.168614107515</v>
       </c>
-      <c r="M28" s="35">
+      <c r="M28" s="30">
         <f>+M8</f>
         <v>28412.088926355034</v>
       </c>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="E29" s="35">
+      <c r="E29" s="30">
         <f>+E12</f>
         <v>25653.620737664289</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="30">
         <f>+I12</f>
         <v>28419.477029887752</v>
       </c>
-      <c r="M29" s="35">
+      <c r="M29" s="30">
         <f>+M12</f>
         <v>29333.632394285651</v>
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="E30" s="35">
+      <c r="E30" s="30">
         <f>+E16</f>
         <v>25535.629724312439</v>
       </c>
-      <c r="I30" s="35">
+      <c r="I30" s="30">
         <f>+I16</f>
         <v>27805.52441776494</v>
       </c>
-      <c r="M30" s="35">
+      <c r="M30" s="30">
         <f>+M16</f>
         <v>30358.748237175794</v>
       </c>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="E31" s="35">
+      <c r="E31" s="30">
         <f>+E20</f>
         <v>25503.985167134437</v>
       </c>
-      <c r="I31" s="35">
+      <c r="I31" s="30">
         <f>+I20</f>
         <v>27994.126519712256</v>
       </c>
-      <c r="M31" s="35">
+      <c r="M31" s="30">
         <f>+M20</f>
         <v>31465.280166833389</v>
       </c>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="E32" s="35">
+      <c r="E32" s="30">
         <f>+E24</f>
         <v>25495.315286140911</v>
       </c>
-      <c r="I32" s="35">
+      <c r="I32" s="30">
         <f>+I24</f>
         <v>27728.886978687318</v>
       </c>
-      <c r="M32" s="35">
+      <c r="M32" s="30">
         <f>+M24</f>
         <v>32624.86478188977</v>
       </c>
     </row>
     <row r="33" spans="4:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="4:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="37">
+      <c r="E34" s="32">
         <v>2023</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="34">
         <v>2024</v>
       </c>
-      <c r="G34" s="39">
+      <c r="G34" s="34">
         <v>2025</v>
       </c>
-      <c r="H34" s="39">
+      <c r="H34" s="34">
         <v>2026</v>
       </c>
-      <c r="I34" s="39">
+      <c r="I34" s="34">
         <v>2027</v>
       </c>
     </row>
     <row r="35" spans="4:9" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="29">
+        <v>26094.765039655078</v>
+      </c>
+      <c r="F35" s="29">
+        <v>25653.620737664289</v>
+      </c>
+      <c r="G35" s="29">
+        <v>25535.629724312439</v>
+      </c>
+      <c r="H35" s="29">
+        <v>25503.985167134437</v>
+      </c>
+      <c r="I35" s="29">
+        <v>25495.315286140911</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="34">
-        <v>26094.765039655078</v>
-      </c>
-      <c r="F35" s="34">
-        <v>25653.620737664289</v>
-      </c>
-      <c r="G35" s="34">
-        <v>25535.629724312439</v>
-      </c>
-      <c r="H35" s="34">
-        <v>25503.985167134437</v>
-      </c>
-      <c r="I35" s="34">
-        <v>25495.315286140911</v>
-      </c>
-    </row>
-    <row r="36" spans="4:9" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="38" t="s">
+      <c r="E36" s="29">
+        <v>26962.168614107515</v>
+      </c>
+      <c r="F36" s="29">
+        <v>28419.477029887752</v>
+      </c>
+      <c r="G36" s="29">
+        <v>27805.52441776494</v>
+      </c>
+      <c r="H36" s="29">
+        <v>27994.126519712256</v>
+      </c>
+      <c r="I36" s="29">
+        <v>27728.886978687318</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="34">
-        <v>26962.168614107515</v>
-      </c>
-      <c r="F36" s="34">
-        <v>28419.477029887752</v>
-      </c>
-      <c r="G36" s="34">
-        <v>27805.52441776494</v>
-      </c>
-      <c r="H36" s="34">
-        <v>27994.126519712256</v>
-      </c>
-      <c r="I36" s="34">
-        <v>27728.886978687318</v>
-      </c>
-    </row>
-    <row r="37" spans="4:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="34">
+      <c r="E37" s="29">
         <v>28412.088926355034</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="29">
         <v>29333.632394285651</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G37" s="29">
         <v>30358.748237175794</v>
       </c>
-      <c r="H37" s="34">
+      <c r="H37" s="29">
         <v>31465.280166833389</v>
       </c>
-      <c r="I37" s="34">
+      <c r="I37" s="29">
         <v>32624.86478188977</v>
       </c>
     </row>
@@ -4807,27 +4796,27 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -4835,87 +4824,87 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="E10" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
     </row>
     <row r="13" spans="1:11" ht="66" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <v>1990</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="11">
         <v>1995</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="11">
         <v>2000</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <v>2005</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <v>2010</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="11">
         <v>2015</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="11">
         <v>2020</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5">
         <v>484</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="6">
         <v>356454</v>
@@ -4940,189 +4929,189 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13">
+        <v>840</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15">
-        <v>840</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="16">
+      <c r="E15" s="14">
         <v>464887</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="14">
         <v>623294</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="14">
         <v>894552</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="14">
         <v>549083</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="14">
         <v>270854</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="14">
         <v>559370</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="14">
         <v>1189312</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="F20" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
     </row>
     <row r="23" spans="1:12" ht="66" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="F23" s="11">
+        <v>1990</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1995</v>
+      </c>
+      <c r="H23" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I23" s="11">
+        <v>2005</v>
+      </c>
+      <c r="J23" s="11">
+        <v>2010</v>
+      </c>
+      <c r="K23" s="11">
+        <v>2015</v>
+      </c>
+      <c r="L23" s="11">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
+        <v>1</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="18">
+        <v>900</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="21">
+        <v>152986157</v>
+      </c>
+      <c r="G24" s="21">
+        <v>161289976</v>
+      </c>
+      <c r="H24" s="21">
+        <v>173230585</v>
+      </c>
+      <c r="I24" s="21">
+        <v>191446828</v>
+      </c>
+      <c r="J24" s="21">
+        <v>220983187</v>
+      </c>
+      <c r="K24" s="21">
+        <v>247958644</v>
+      </c>
+      <c r="L24" s="21">
+        <v>280598105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
+        <v>255</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="13">
-        <v>1990</v>
-      </c>
-      <c r="G23" s="13">
-        <v>1995</v>
-      </c>
-      <c r="H23" s="13">
-        <v>2000</v>
-      </c>
-      <c r="I23" s="13">
-        <v>2005</v>
-      </c>
-      <c r="J23" s="13">
-        <v>2010</v>
-      </c>
-      <c r="K23" s="13">
-        <v>2015</v>
-      </c>
-      <c r="L23" s="13">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="22">
-        <v>1</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="22">
-        <v>900</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="25">
-        <v>152986157</v>
-      </c>
-      <c r="G24" s="25">
-        <v>161289976</v>
-      </c>
-      <c r="H24" s="25">
-        <v>173230585</v>
-      </c>
-      <c r="I24" s="25">
-        <v>191446828</v>
-      </c>
-      <c r="J24" s="25">
-        <v>220983187</v>
-      </c>
-      <c r="K24" s="25">
-        <v>247958644</v>
-      </c>
-      <c r="L24" s="25">
-        <v>280598105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="15">
-        <v>255</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="C25" s="16">
+        <v>33</v>
+      </c>
+      <c r="D25" s="13">
+        <v>840</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="18">
-        <v>33</v>
-      </c>
-      <c r="D25" s="15">
-        <v>840</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="16">
+      <c r="F25" s="14">
         <v>23251026</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="14">
         <v>28451053</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="14">
         <v>34814053</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="14">
         <v>39258293</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="14">
         <v>44183643</v>
       </c>
-      <c r="K25" s="16">
+      <c r="K25" s="14">
         <v>48178877</v>
       </c>
-      <c r="L25" s="16">
+      <c r="L25" s="14">
         <v>50632836</v>
       </c>
     </row>
@@ -5131,14 +5120,14 @@
         <v>232</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="17"/>
+        <v>5</v>
+      </c>
+      <c r="C26" s="15"/>
       <c r="D26" s="5">
         <v>484</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" s="6">
         <v>695674</v>
@@ -5184,19 +5173,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>